<commit_message>
update Gatton2014-16 observed phenology
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/Gatton2014_2016.xlsx
+++ b/Tests/Validation/Wheat/Gatton2014_2016.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\Wheat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4DE763-E805-493C-957B-BE72B66AA096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00E4E4A-A439-48B7-96A8-F880A2B74D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3558" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3596" uniqueCount="355">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1491,13 +1491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V2689"/>
+  <dimension ref="A1:S2689"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2546" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2667" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:S1048576"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28521,497 +28521,630 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2395" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2395" t="s">
+    <row r="2395" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2395" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C2395" t="s">
+      <c r="B2395" s="5"/>
+      <c r="C2395" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="D2395">
+      <c r="D2395" s="4">
         <v>11</v>
       </c>
-      <c r="F2395">
-        <v>57</v>
-      </c>
-      <c r="I2395">
-        <v>69</v>
-      </c>
-      <c r="J2395">
-        <v>85</v>
-      </c>
-      <c r="K2395">
-        <v>92</v>
-      </c>
-      <c r="L2395">
+      <c r="F2395" s="4">
+        <v>113</v>
+      </c>
+      <c r="G2395" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2395" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2395" s="4">
+        <v>125</v>
+      </c>
+      <c r="J2395" s="4">
+        <v>141</v>
+      </c>
+      <c r="K2395" s="4">
+        <v>148</v>
+      </c>
+      <c r="L2395" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2396" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2396" s="5"/>
+      <c r="C2396" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2396" s="4">
+        <v>9</v>
+      </c>
+      <c r="F2396" s="4">
+        <v>104</v>
+      </c>
+      <c r="G2396" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2396" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2396" s="4">
+        <v>114</v>
+      </c>
+      <c r="J2396" s="4">
+        <v>130</v>
+      </c>
+      <c r="K2396" s="4">
+        <v>138</v>
+      </c>
+      <c r="L2396" s="4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2397" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2397" s="5"/>
+      <c r="C2397" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2397" s="4">
+        <v>11</v>
+      </c>
+      <c r="F2397" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2397" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2397" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2397" s="4">
+        <v>131</v>
+      </c>
+      <c r="J2397" s="4">
+        <v>152</v>
+      </c>
+      <c r="K2397" s="4">
+        <v>159</v>
+      </c>
+      <c r="L2397" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2398" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2398" s="5"/>
+      <c r="C2398" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2398" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2398" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2398" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2398" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2398" s="4">
+        <v>123</v>
+      </c>
+      <c r="J2398" s="4">
+        <v>139</v>
+      </c>
+      <c r="K2398" s="4">
+        <v>148</v>
+      </c>
+      <c r="L2398" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2399" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2399" s="5"/>
+      <c r="C2399" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2399" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2399" s="4">
+        <v>112</v>
+      </c>
+      <c r="G2399" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2399" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2399" s="4">
+        <v>128</v>
+      </c>
+      <c r="J2399" s="4">
+        <v>142</v>
+      </c>
+      <c r="K2399" s="4">
+        <v>150</v>
+      </c>
+      <c r="L2399" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2400" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2400" s="5"/>
+      <c r="C2400" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2400" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2400" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2400" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2400" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2400" s="4">
+        <v>125</v>
+      </c>
+      <c r="J2400" s="4">
+        <v>140</v>
+      </c>
+      <c r="K2400" s="4">
+        <v>148</v>
+      </c>
+      <c r="L2400" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2401" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2401" s="5"/>
+      <c r="C2401" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2401" s="4">
+        <v>9</v>
+      </c>
+      <c r="F2401" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2401" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2401" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2401" s="4">
+        <v>118</v>
+      </c>
+      <c r="J2401" s="4">
+        <v>133</v>
+      </c>
+      <c r="K2401" s="4">
+        <v>142</v>
+      </c>
+      <c r="L2401" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2402" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B2402" s="5"/>
+      <c r="C2402" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2402" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2402" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2402" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2402" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2402" s="4">
+        <v>128</v>
+      </c>
+      <c r="J2402" s="4">
+        <v>142</v>
+      </c>
+      <c r="K2402" s="4">
+        <v>151</v>
+      </c>
+      <c r="L2402" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2403" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2403" s="5"/>
+      <c r="C2403" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2403" s="4">
+        <v>9.5</v>
+      </c>
+      <c r="F2403" s="4">
+        <v>107</v>
+      </c>
+      <c r="G2403" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2403" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2403" s="4">
+        <v>118</v>
+      </c>
+      <c r="J2403" s="4">
+        <v>133</v>
+      </c>
+      <c r="K2403" s="4">
+        <v>140</v>
+      </c>
+      <c r="L2403" s="4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2404" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2404" s="5"/>
+      <c r="C2404" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2404" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2404" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2404" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2404" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2404" s="4">
+        <v>125</v>
+      </c>
+      <c r="J2404" s="4">
+        <v>141</v>
+      </c>
+      <c r="K2404" s="4">
+        <v>148</v>
+      </c>
+      <c r="L2404" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2405" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2405" s="5"/>
+      <c r="C2405" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2405" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2405" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2405" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2405" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2405" s="4">
+        <v>124</v>
+      </c>
+      <c r="J2405" s="4">
+        <v>140</v>
+      </c>
+      <c r="K2405" s="4">
+        <v>148</v>
+      </c>
+      <c r="L2405" s="4">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2406" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2406" s="5"/>
+      <c r="C2406" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2406" s="4">
+        <v>9</v>
+      </c>
+      <c r="F2406" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2406" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2406" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2406" s="4">
+        <v>120</v>
+      </c>
+      <c r="J2406" s="4">
+        <v>134</v>
+      </c>
+      <c r="K2406" s="4">
+        <v>141</v>
+      </c>
+      <c r="L2406" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2407" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2407" s="5"/>
+      <c r="C2407" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2407" s="4">
+        <v>9</v>
+      </c>
+      <c r="F2407" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2407" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2407" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2407" s="4">
+        <v>119</v>
+      </c>
+      <c r="J2407" s="4">
+        <v>133</v>
+      </c>
+      <c r="K2407" s="4">
+        <v>141</v>
+      </c>
+      <c r="L2407" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2408" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2408" s="5"/>
+      <c r="C2408" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2408" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2408" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2408" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2408" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2408" s="4">
+        <v>120</v>
+      </c>
+      <c r="J2408" s="4">
+        <v>135</v>
+      </c>
+      <c r="K2408" s="4">
+        <v>140</v>
+      </c>
+      <c r="L2408" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2409" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2409" s="5"/>
+      <c r="C2409" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2409" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="F2409" s="4">
+        <v>105</v>
+      </c>
+      <c r="G2409" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2409" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2409" s="4">
+        <v>117</v>
+      </c>
+      <c r="J2409" s="4">
+        <v>134</v>
+      </c>
+      <c r="K2409" s="4">
+        <v>141</v>
+      </c>
+      <c r="L2409" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2410" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2410" s="5"/>
+      <c r="C2410" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2410" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="F2410" s="4">
+        <v>112</v>
+      </c>
+      <c r="G2410" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2410" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2410" s="4">
+        <v>124</v>
+      </c>
+      <c r="J2410" s="4">
+        <v>145</v>
+      </c>
+      <c r="K2410" s="4">
+        <v>150</v>
+      </c>
+      <c r="L2410" s="4">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2411" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2411" s="5"/>
+      <c r="C2411" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2411" s="4">
+        <v>11</v>
+      </c>
+      <c r="F2411" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2411" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2411" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2411" s="4">
+        <v>125</v>
+      </c>
+      <c r="J2411" s="4">
+        <v>139</v>
+      </c>
+      <c r="K2411" s="4">
+        <v>145</v>
+      </c>
+      <c r="L2411" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2412" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2412" s="5"/>
+      <c r="C2412" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="D2412" s="4">
+        <v>10</v>
+      </c>
+      <c r="F2412" s="4">
+        <v>106</v>
+      </c>
+      <c r="G2412" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2412" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2412" s="4">
         <v>127</v>
       </c>
-    </row>
-    <row r="2396" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2396" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2396" t="s">
+      <c r="J2412" s="4">
+        <v>141</v>
+      </c>
+      <c r="K2412" s="4">
+        <v>148</v>
+      </c>
+      <c r="L2412" s="4">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2413" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2413" s="5"/>
+      <c r="C2413" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="D2396">
-        <v>9</v>
-      </c>
-      <c r="F2396">
-        <v>48</v>
-      </c>
-      <c r="I2396">
-        <v>58</v>
-      </c>
-      <c r="J2396">
-        <v>74</v>
-      </c>
-      <c r="K2396">
-        <v>82</v>
-      </c>
-      <c r="L2396">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2397" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2397" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2397" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2397">
-        <v>11</v>
-      </c>
-      <c r="F2397">
-        <v>50</v>
-      </c>
-      <c r="I2397">
-        <v>75</v>
-      </c>
-      <c r="J2397">
-        <v>96</v>
-      </c>
-      <c r="K2397">
-        <v>103</v>
-      </c>
-      <c r="L2397" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2398" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2398" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2398" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2398">
+      <c r="D2413" s="4">
         <v>10</v>
       </c>
-      <c r="F2398">
-        <v>50</v>
-      </c>
-      <c r="I2398">
-        <v>67</v>
-      </c>
-      <c r="J2398">
-        <v>83</v>
-      </c>
-      <c r="K2398">
-        <v>92</v>
-      </c>
-      <c r="L2398">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2399" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2399" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2399" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2399">
-        <v>10</v>
-      </c>
-      <c r="F2399">
-        <v>56</v>
-      </c>
-      <c r="I2399">
-        <v>72</v>
-      </c>
-      <c r="J2399">
-        <v>86</v>
-      </c>
-      <c r="K2399">
-        <v>94</v>
-      </c>
-      <c r="L2399">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2400" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2400" t="s">
-        <v>108</v>
-      </c>
-      <c r="C2400" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2400">
-        <v>10</v>
-      </c>
-      <c r="F2400">
-        <v>50</v>
-      </c>
-      <c r="I2400">
-        <v>69</v>
-      </c>
-      <c r="J2400">
-        <v>84</v>
-      </c>
-      <c r="K2400">
-        <v>92</v>
-      </c>
-      <c r="L2400">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2401" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2401" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2401" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2401">
-        <v>9</v>
-      </c>
-      <c r="F2401">
-        <v>50</v>
-      </c>
-      <c r="I2401">
-        <v>62</v>
-      </c>
-      <c r="J2401">
-        <v>77</v>
-      </c>
-      <c r="K2401">
-        <v>86</v>
-      </c>
-      <c r="L2401" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2402" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2402" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2402" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2402">
-        <v>10</v>
-      </c>
-      <c r="F2402">
-        <v>50</v>
-      </c>
-      <c r="I2402">
-        <v>72</v>
-      </c>
-      <c r="J2402">
-        <v>86</v>
-      </c>
-      <c r="K2402">
-        <v>95</v>
-      </c>
-      <c r="L2402">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2403" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2403" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2403" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2403">
-        <v>9.5</v>
-      </c>
-      <c r="F2403">
-        <v>51</v>
-      </c>
-      <c r="I2403">
-        <v>62</v>
-      </c>
-      <c r="J2403">
-        <v>77</v>
-      </c>
-      <c r="K2403">
-        <v>84</v>
-      </c>
-      <c r="L2403">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2404" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2404" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2404" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2404">
-        <v>10</v>
-      </c>
-      <c r="F2404">
-        <v>50</v>
-      </c>
-      <c r="I2404">
-        <v>69</v>
-      </c>
-      <c r="J2404">
-        <v>85</v>
-      </c>
-      <c r="K2404">
-        <v>92</v>
-      </c>
-      <c r="L2404">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2405" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2405" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2405" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2405">
-        <v>10</v>
-      </c>
-      <c r="F2405">
-        <v>50</v>
-      </c>
-      <c r="I2405">
-        <v>68</v>
-      </c>
-      <c r="J2405">
-        <v>84</v>
-      </c>
-      <c r="K2405">
-        <v>92</v>
-      </c>
-      <c r="L2405">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2406" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2406" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2406" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2406">
-        <v>9</v>
-      </c>
-      <c r="F2406">
-        <v>50</v>
-      </c>
-      <c r="I2406">
-        <v>64</v>
-      </c>
-      <c r="J2406">
-        <v>78</v>
-      </c>
-      <c r="K2406">
-        <v>85</v>
-      </c>
-      <c r="L2406">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2407" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2407" t="s">
-        <v>78</v>
-      </c>
-      <c r="C2407" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2407">
-        <v>9</v>
-      </c>
-      <c r="F2407">
-        <v>50</v>
-      </c>
-      <c r="I2407">
-        <v>63</v>
-      </c>
-      <c r="J2407">
-        <v>77</v>
-      </c>
-      <c r="K2407">
-        <v>85</v>
-      </c>
-      <c r="L2407" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2408" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2408" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2408" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2408">
-        <v>10</v>
-      </c>
-      <c r="F2408">
-        <v>50</v>
-      </c>
-      <c r="I2408">
-        <v>64</v>
-      </c>
-      <c r="J2408">
-        <v>79</v>
-      </c>
-      <c r="K2408">
-        <v>84</v>
-      </c>
-      <c r="L2408" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2409" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2409" t="s">
-        <v>340</v>
-      </c>
-      <c r="C2409" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2409">
-        <v>10.5</v>
-      </c>
-      <c r="F2409">
-        <v>49</v>
-      </c>
-      <c r="I2409">
-        <v>61</v>
-      </c>
-      <c r="J2409">
-        <v>78</v>
-      </c>
-      <c r="K2409">
-        <v>85</v>
-      </c>
-      <c r="L2409" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2410" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2410" t="s">
+      <c r="F2413" s="4">
         <v>105</v>
       </c>
-      <c r="C2410" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2410">
-        <v>10.5</v>
-      </c>
-      <c r="F2410">
-        <v>56</v>
-      </c>
-      <c r="I2410">
-        <v>68</v>
-      </c>
-      <c r="J2410">
-        <v>89</v>
-      </c>
-      <c r="K2410">
-        <v>94</v>
-      </c>
-      <c r="L2410">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2411" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2411" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2411" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2411">
-        <v>11</v>
-      </c>
-      <c r="F2411">
-        <v>50</v>
-      </c>
-      <c r="I2411">
-        <v>69</v>
-      </c>
-      <c r="J2411">
-        <v>83</v>
-      </c>
-      <c r="K2411">
-        <v>89</v>
-      </c>
-      <c r="L2411" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2412" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2412" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2412" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2412">
-        <v>10</v>
-      </c>
-      <c r="F2412">
-        <v>50</v>
-      </c>
-      <c r="I2412">
-        <v>71</v>
-      </c>
-      <c r="J2412">
-        <v>85</v>
-      </c>
-      <c r="K2412">
-        <v>92</v>
-      </c>
-      <c r="L2412">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2413" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2413" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2413" t="s">
-        <v>330</v>
-      </c>
-      <c r="D2413">
-        <v>10</v>
-      </c>
-      <c r="F2413">
-        <v>49</v>
-      </c>
-      <c r="I2413">
-        <v>59</v>
-      </c>
-      <c r="J2413">
-        <v>76</v>
-      </c>
-      <c r="K2413">
-        <v>82</v>
-      </c>
-      <c r="L2413" t="s">
+      <c r="G2413" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2413" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I2413" s="4">
+        <v>115</v>
+      </c>
+      <c r="J2413" s="4">
+        <v>132</v>
+      </c>
+      <c r="K2413" s="4">
+        <v>138</v>
+      </c>
+      <c r="L2413" s="4" t="s">
         <v>337</v>
       </c>
     </row>
@@ -32837,7 +32970,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2561" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2561" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2561" t="s">
         <v>42</v>
       </c>
@@ -32863,7 +32996,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2562" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2562" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2562" t="s">
         <v>46</v>
       </c>
@@ -32889,7 +33022,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2563" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2563" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2563" t="s">
         <v>51</v>
       </c>
@@ -32915,7 +33048,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2564" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2564" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2564" t="s">
         <v>70</v>
       </c>
@@ -32941,7 +33074,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2565" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2565" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2565" s="4" t="s">
         <v>111</v>
       </c>
@@ -32953,7 +33086,7 @@
         <v>337</v>
       </c>
       <c r="F2565" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2565" s="4" t="s">
         <v>337</v>
@@ -32962,27 +33095,23 @@
         <v>337</v>
       </c>
       <c r="I2565" s="4">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="J2565" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="K2565" s="4">
-        <v>195</v>
+        <v>139</v>
       </c>
       <c r="L2565" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="U2565" s="4" t="str">
-        <f t="shared" ref="N2565:AC2580" si="0">IF(N2565="","",N2565+56)</f>
+      <c r="S2565" s="4" t="str">
+        <f t="shared" ref="N2565:W2565" si="0">IF(L2565="","",L2565-56)</f>
         <v/>
       </c>
-      <c r="V2565" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="2566" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2566" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2566" s="4" t="s">
         <v>347</v>
       </c>
@@ -32994,7 +33123,7 @@
         <v>337</v>
       </c>
       <c r="F2566" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2566" s="4" t="s">
         <v>337</v>
@@ -33003,19 +33132,19 @@
         <v>337</v>
       </c>
       <c r="I2566" s="4">
-        <v>180</v>
+        <v>124</v>
       </c>
       <c r="J2566" s="4">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="K2566" s="4">
-        <v>199</v>
+        <v>143</v>
       </c>
       <c r="L2566" s="4">
         <v>237</v>
       </c>
     </row>
-    <row r="2567" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2567" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2567" s="4" t="s">
         <v>80</v>
       </c>
@@ -33027,7 +33156,7 @@
         <v>337</v>
       </c>
       <c r="F2567" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="G2567" s="4" t="s">
         <v>337</v>
@@ -33036,19 +33165,19 @@
         <v>337</v>
       </c>
       <c r="I2567" s="4">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="J2567" s="4">
-        <v>206</v>
+        <v>150</v>
       </c>
       <c r="K2567" s="4">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="L2567" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2568" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2568" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2568" s="4" t="s">
         <v>104</v>
       </c>
@@ -33060,7 +33189,7 @@
         <v>337</v>
       </c>
       <c r="F2568" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2568" s="4" t="s">
         <v>337</v>
@@ -33069,19 +33198,19 @@
         <v>337</v>
       </c>
       <c r="I2568" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="J2568" s="4">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="K2568" s="4">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="L2568" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2569" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2569" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2569" s="4" t="s">
         <v>83</v>
       </c>
@@ -33093,7 +33222,7 @@
         <v>337</v>
       </c>
       <c r="F2569" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2569" s="4" t="s">
         <v>337</v>
@@ -33102,19 +33231,19 @@
         <v>337</v>
       </c>
       <c r="I2569" s="4">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="J2569" s="4">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="K2569" s="4">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="L2569" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2570" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2570" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2570" s="4" t="s">
         <v>96</v>
       </c>
@@ -33126,7 +33255,7 @@
         <v>337</v>
       </c>
       <c r="F2570" s="4">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="G2570" s="4" t="s">
         <v>337</v>
@@ -33135,19 +33264,19 @@
         <v>337</v>
       </c>
       <c r="I2570" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="J2570" s="4">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="K2570" s="4">
-        <v>199</v>
+        <v>143</v>
       </c>
       <c r="L2570" s="4">
         <v>239</v>
       </c>
     </row>
-    <row r="2571" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2571" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2571" s="4" t="s">
         <v>316</v>
       </c>
@@ -33159,7 +33288,7 @@
         <v>337</v>
       </c>
       <c r="F2571" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="G2571" s="4" t="s">
         <v>337</v>
@@ -33168,19 +33297,19 @@
         <v>337</v>
       </c>
       <c r="I2571" s="4">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="J2571" s="4">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="K2571" s="4">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="L2571" s="4">
         <v>236</v>
       </c>
     </row>
-    <row r="2572" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2572" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2572" s="4" t="s">
         <v>85</v>
       </c>
@@ -33192,7 +33321,7 @@
         <v>337</v>
       </c>
       <c r="F2572" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2572" s="4" t="s">
         <v>337</v>
@@ -33201,19 +33330,19 @@
         <v>337</v>
       </c>
       <c r="I2572" s="4">
-        <v>194</v>
+        <v>138</v>
       </c>
       <c r="J2572" s="4">
-        <v>208</v>
+        <v>152</v>
       </c>
       <c r="K2572" s="4">
-        <v>215</v>
+        <v>159</v>
       </c>
       <c r="L2572" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2573" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2573" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2573" s="4" t="s">
         <v>317</v>
       </c>
@@ -33225,7 +33354,7 @@
         <v>337</v>
       </c>
       <c r="F2573" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2573" s="4" t="s">
         <v>337</v>
@@ -33234,19 +33363,19 @@
         <v>337</v>
       </c>
       <c r="I2573" s="4">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="J2573" s="4">
-        <v>191</v>
+        <v>135</v>
       </c>
       <c r="K2573" s="4">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="L2573" s="4">
         <v>236</v>
       </c>
     </row>
-    <row r="2574" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2574" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2574" s="4" t="s">
         <v>97</v>
       </c>
@@ -33258,7 +33387,7 @@
         <v>337</v>
       </c>
       <c r="F2574" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2574" s="4" t="s">
         <v>337</v>
@@ -33267,19 +33396,19 @@
         <v>337</v>
       </c>
       <c r="I2574" s="4">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="J2574" s="4">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="K2574" s="4">
-        <v>203</v>
+        <v>147</v>
       </c>
       <c r="L2574" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2575" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2575" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2575" s="4" t="s">
         <v>77</v>
       </c>
@@ -33291,7 +33420,7 @@
         <v>337</v>
       </c>
       <c r="F2575" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2575" s="4" t="s">
         <v>337</v>
@@ -33300,19 +33429,19 @@
         <v>337</v>
       </c>
       <c r="I2575" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="J2575" s="4">
-        <v>208</v>
+        <v>152</v>
       </c>
       <c r="K2575" s="4">
-        <v>213</v>
+        <v>157</v>
       </c>
       <c r="L2575" s="4" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="2576" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2576" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2576" s="4" t="s">
         <v>103</v>
       </c>
@@ -33324,7 +33453,7 @@
         <v>337</v>
       </c>
       <c r="F2576" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="G2576" s="4" t="s">
         <v>337</v>
@@ -33333,13 +33462,13 @@
         <v>337</v>
       </c>
       <c r="I2576" s="4">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="J2576" s="4">
-        <v>202</v>
+        <v>146</v>
       </c>
       <c r="K2576" s="4">
-        <v>209</v>
+        <v>153</v>
       </c>
       <c r="L2576" s="4">
         <v>240</v>
@@ -33357,7 +33486,7 @@
         <v>337</v>
       </c>
       <c r="F2577" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="G2577" s="4" t="s">
         <v>337</v>
@@ -33366,13 +33495,13 @@
         <v>337</v>
       </c>
       <c r="I2577" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="J2577" s="4">
-        <v>198</v>
+        <v>142</v>
       </c>
       <c r="K2577" s="4">
-        <v>205</v>
+        <v>149</v>
       </c>
       <c r="L2577" s="4">
         <v>240</v>
@@ -33390,7 +33519,7 @@
         <v>337</v>
       </c>
       <c r="F2578" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2578" s="4" t="s">
         <v>337</v>
@@ -33399,13 +33528,13 @@
         <v>337</v>
       </c>
       <c r="I2578" s="4">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="J2578" s="4">
-        <v>193</v>
+        <v>137</v>
       </c>
       <c r="K2578" s="4">
-        <v>199</v>
+        <v>143</v>
       </c>
       <c r="L2578" s="4" t="s">
         <v>337</v>
@@ -33423,7 +33552,7 @@
         <v>337</v>
       </c>
       <c r="F2579" s="4">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="G2579" s="4" t="s">
         <v>337</v>
@@ -33432,13 +33561,13 @@
         <v>337</v>
       </c>
       <c r="I2579" s="4">
-        <v>200</v>
+        <v>144</v>
       </c>
       <c r="J2579" s="4">
-        <v>209</v>
+        <v>153</v>
       </c>
       <c r="K2579" s="4">
-        <v>216</v>
+        <v>160</v>
       </c>
       <c r="L2579" s="4" t="s">
         <v>337</v>
@@ -33456,7 +33585,7 @@
         <v>337</v>
       </c>
       <c r="F2580" s="4">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="G2580" s="4" t="s">
         <v>337</v>
@@ -33465,13 +33594,13 @@
         <v>337</v>
       </c>
       <c r="I2580" s="4">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="J2580" s="4">
-        <v>201</v>
+        <v>145</v>
       </c>
       <c r="K2580" s="4">
-        <v>208</v>
+        <v>152</v>
       </c>
       <c r="L2580" s="4" t="s">
         <v>337</v>
@@ -33489,7 +33618,7 @@
         <v>337</v>
       </c>
       <c r="F2581" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2581" s="4" t="s">
         <v>337</v>
@@ -33498,13 +33627,13 @@
         <v>337</v>
       </c>
       <c r="I2581" s="4">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="J2581" s="4">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="K2581" s="4">
-        <v>199</v>
+        <v>143</v>
       </c>
       <c r="L2581" s="4" t="s">
         <v>337</v>
@@ -33522,7 +33651,7 @@
         <v>337</v>
       </c>
       <c r="F2582" s="4">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="G2582" s="4" t="s">
         <v>337</v>
@@ -33531,13 +33660,13 @@
         <v>337</v>
       </c>
       <c r="I2582" s="4">
-        <v>183</v>
+        <v>127</v>
       </c>
       <c r="J2582" s="4">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="K2582" s="4">
-        <v>205</v>
+        <v>149</v>
       </c>
       <c r="L2582" s="4">
         <v>237</v>
@@ -33555,7 +33684,7 @@
         <v>337</v>
       </c>
       <c r="F2583" s="4">
-        <v>183</v>
+        <v>127</v>
       </c>
       <c r="G2583" s="4" t="s">
         <v>337</v>
@@ -33564,13 +33693,13 @@
         <v>337</v>
       </c>
       <c r="I2583" s="4">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="J2583" s="4">
-        <v>206</v>
+        <v>150</v>
       </c>
       <c r="K2583" s="4">
-        <v>210</v>
+        <v>154</v>
       </c>
       <c r="L2583" s="4">
         <v>240</v>
@@ -33588,7 +33717,7 @@
         <v>337</v>
       </c>
       <c r="F2584" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2584" s="4" t="s">
         <v>337</v>
@@ -33597,13 +33726,13 @@
         <v>337</v>
       </c>
       <c r="I2584" s="4">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="J2584" s="4">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="K2584" s="4">
-        <v>197</v>
+        <v>141</v>
       </c>
       <c r="L2584" s="4">
         <v>236</v>
@@ -33621,7 +33750,7 @@
         <v>337</v>
       </c>
       <c r="F2585" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="G2585" s="4" t="s">
         <v>337</v>
@@ -33630,13 +33759,13 @@
         <v>337</v>
       </c>
       <c r="I2585" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="J2585" s="4">
-        <v>201</v>
+        <v>145</v>
       </c>
       <c r="K2585" s="4">
-        <v>207</v>
+        <v>151</v>
       </c>
       <c r="L2585" s="4">
         <v>239</v>
@@ -33654,7 +33783,7 @@
         <v>337</v>
       </c>
       <c r="F2586" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2586" s="4" t="s">
         <v>337</v>
@@ -33663,13 +33792,13 @@
         <v>337</v>
       </c>
       <c r="I2586" s="4">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="J2586" s="4">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="K2586" s="4">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="L2586" s="4" t="s">
         <v>337</v>
@@ -33687,7 +33816,7 @@
         <v>337</v>
       </c>
       <c r="F2587" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2587" s="4" t="s">
         <v>337</v>
@@ -33696,13 +33825,13 @@
         <v>337</v>
       </c>
       <c r="I2587" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2587" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="K2587" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="L2587" s="4">
         <v>226</v>
@@ -33720,7 +33849,7 @@
         <v>337</v>
       </c>
       <c r="F2588" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2588" s="4" t="s">
         <v>337</v>
@@ -33729,13 +33858,13 @@
         <v>337</v>
       </c>
       <c r="I2588" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2588" s="4">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="K2588" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2588" s="4">
         <v>225</v>
@@ -33753,7 +33882,7 @@
         <v>337</v>
       </c>
       <c r="F2589" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2589" s="4" t="s">
         <v>337</v>
@@ -33762,13 +33891,13 @@
         <v>337</v>
       </c>
       <c r="I2589" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="J2589" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="K2589" s="4">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="L2589" s="4" t="s">
         <v>337</v>
@@ -33786,7 +33915,7 @@
         <v>337</v>
       </c>
       <c r="F2590" s="4">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="G2590" s="4" t="s">
         <v>337</v>
@@ -33795,13 +33924,13 @@
         <v>337</v>
       </c>
       <c r="I2590" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="J2590" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="K2590" s="4">
-        <v>191</v>
+        <v>135</v>
       </c>
       <c r="L2590" s="4" t="s">
         <v>337</v>
@@ -33819,7 +33948,7 @@
         <v>337</v>
       </c>
       <c r="F2591" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2591" s="4" t="s">
         <v>337</v>
@@ -33828,13 +33957,13 @@
         <v>337</v>
       </c>
       <c r="I2591" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2591" s="4">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="K2591" s="4">
-        <v>185</v>
+        <v>129</v>
       </c>
       <c r="L2591" s="4">
         <v>226</v>
@@ -33852,7 +33981,7 @@
         <v>337</v>
       </c>
       <c r="F2592" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2592" s="4" t="s">
         <v>337</v>
@@ -33861,13 +33990,13 @@
         <v>337</v>
       </c>
       <c r="I2592" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2592" s="4">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="K2592" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2592" s="4">
         <v>226</v>
@@ -33885,7 +34014,7 @@
         <v>337</v>
       </c>
       <c r="F2593" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2593" s="4" t="s">
         <v>337</v>
@@ -33894,13 +34023,13 @@
         <v>337</v>
       </c>
       <c r="I2593" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2593" s="4">
-        <v>169</v>
+        <v>113</v>
       </c>
       <c r="K2593" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2593" s="4">
         <v>225</v>
@@ -33918,7 +34047,7 @@
         <v>337</v>
       </c>
       <c r="F2594" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2594" s="4" t="s">
         <v>337</v>
@@ -33927,13 +34056,13 @@
         <v>337</v>
       </c>
       <c r="I2594" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2594" s="4">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="K2594" s="4">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="L2594" s="4">
         <v>226</v>
@@ -33951,7 +34080,7 @@
         <v>337</v>
       </c>
       <c r="F2595" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2595" s="4" t="s">
         <v>337</v>
@@ -33960,13 +34089,13 @@
         <v>337</v>
       </c>
       <c r="I2595" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2595" s="4">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="K2595" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2595" s="4">
         <v>226</v>
@@ -33984,7 +34113,7 @@
         <v>337</v>
       </c>
       <c r="F2596" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2596" s="4" t="s">
         <v>337</v>
@@ -33993,13 +34122,13 @@
         <v>337</v>
       </c>
       <c r="I2596" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2596" s="4">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="K2596" s="4">
-        <v>186</v>
+        <v>130</v>
       </c>
       <c r="L2596" s="4">
         <v>226</v>
@@ -34017,7 +34146,7 @@
         <v>337</v>
       </c>
       <c r="F2597" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2597" s="4" t="s">
         <v>337</v>
@@ -34026,13 +34155,13 @@
         <v>337</v>
       </c>
       <c r="I2597" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2597" s="4">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="K2597" s="4">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="L2597" s="4">
         <v>225</v>
@@ -34050,7 +34179,7 @@
         <v>337</v>
       </c>
       <c r="F2598" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2598" s="4" t="s">
         <v>337</v>
@@ -34059,13 +34188,13 @@
         <v>337</v>
       </c>
       <c r="I2598" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2598" s="4">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="K2598" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="L2598" s="4">
         <v>226</v>
@@ -34083,7 +34212,7 @@
         <v>337</v>
       </c>
       <c r="F2599" s="4">
-        <v>158</v>
+        <v>102</v>
       </c>
       <c r="G2599" s="4" t="s">
         <v>337</v>
@@ -34092,13 +34221,13 @@
         <v>337</v>
       </c>
       <c r="I2599" s="4">
-        <v>164</v>
+        <v>108</v>
       </c>
       <c r="J2599" s="4">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="K2599" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2599" s="4">
         <v>226</v>
@@ -34116,7 +34245,7 @@
         <v>337</v>
       </c>
       <c r="F2600" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2600" s="4" t="s">
         <v>337</v>
@@ -34125,13 +34254,13 @@
         <v>337</v>
       </c>
       <c r="I2600" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2600" s="4">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="K2600" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2600" s="4">
         <v>226</v>
@@ -34149,7 +34278,7 @@
         <v>337</v>
       </c>
       <c r="F2601" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2601" s="4" t="s">
         <v>337</v>
@@ -34158,13 +34287,13 @@
         <v>337</v>
       </c>
       <c r="I2601" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2601" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="K2601" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="L2601" s="4">
         <v>226</v>
@@ -34182,7 +34311,7 @@
         <v>337</v>
       </c>
       <c r="F2602" s="4">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="G2602" s="4" t="s">
         <v>337</v>
@@ -34191,13 +34320,13 @@
         <v>337</v>
       </c>
       <c r="I2602" s="4">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="J2602" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="K2602" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2602" s="4">
         <v>225</v>
@@ -34215,7 +34344,7 @@
         <v>337</v>
       </c>
       <c r="F2603" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2603" s="4" t="s">
         <v>337</v>
@@ -34224,13 +34353,13 @@
         <v>337</v>
       </c>
       <c r="I2603" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2603" s="4">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="K2603" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2603" s="4">
         <v>225</v>
@@ -34248,7 +34377,7 @@
         <v>337</v>
       </c>
       <c r="F2604" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2604" s="4" t="s">
         <v>337</v>
@@ -34257,13 +34386,13 @@
         <v>337</v>
       </c>
       <c r="I2604" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="J2604" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="K2604" s="4">
-        <v>189</v>
+        <v>133</v>
       </c>
       <c r="L2604" s="4" t="s">
         <v>337</v>
@@ -34281,7 +34410,7 @@
         <v>337</v>
       </c>
       <c r="F2605" s="4">
-        <v>142</v>
+        <v>86</v>
       </c>
       <c r="G2605" s="4" t="s">
         <v>337</v>
@@ -34290,13 +34419,13 @@
         <v>337</v>
       </c>
       <c r="I2605" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="J2605" s="4">
-        <v>168</v>
+        <v>112</v>
       </c>
       <c r="K2605" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2605" s="4">
         <v>225</v>
@@ -34314,7 +34443,7 @@
         <v>337</v>
       </c>
       <c r="F2606" s="4">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="G2606" s="4" t="s">
         <v>337</v>
@@ -34323,13 +34452,13 @@
         <v>337</v>
       </c>
       <c r="I2606" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="J2606" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="K2606" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="L2606" s="4">
         <v>226</v>
@@ -34347,7 +34476,7 @@
         <v>337</v>
       </c>
       <c r="F2607" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2607" s="4" t="s">
         <v>337</v>
@@ -34356,13 +34485,13 @@
         <v>337</v>
       </c>
       <c r="I2607" s="4">
-        <v>160</v>
+        <v>104</v>
       </c>
       <c r="J2607" s="4">
-        <v>172</v>
+        <v>116</v>
       </c>
       <c r="K2607" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="L2607" s="4">
         <v>225</v>
@@ -34380,7 +34509,7 @@
         <v>337</v>
       </c>
       <c r="F2608" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2608" s="4" t="s">
         <v>337</v>
@@ -34389,13 +34518,13 @@
         <v>337</v>
       </c>
       <c r="I2608" s="4">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="J2608" s="4">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="K2608" s="4">
-        <v>187</v>
+        <v>131</v>
       </c>
       <c r="L2608" s="4">
         <v>226</v>
@@ -34413,7 +34542,7 @@
         <v>337</v>
       </c>
       <c r="F2609" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2609" s="4" t="s">
         <v>337</v>
@@ -34422,13 +34551,13 @@
         <v>337</v>
       </c>
       <c r="I2609" s="4">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="J2609" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="K2609" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="L2609" s="4" t="s">
         <v>337</v>
@@ -34446,7 +34575,7 @@
         <v>337</v>
       </c>
       <c r="F2610" s="4">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="G2610" s="4" t="s">
         <v>337</v>
@@ -34455,13 +34584,13 @@
         <v>337</v>
       </c>
       <c r="I2610" s="4">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="J2610" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="K2610" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="L2610" s="4" t="s">
         <v>337</v>
@@ -34479,7 +34608,7 @@
         <v>337</v>
       </c>
       <c r="F2611" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2611" s="4" t="s">
         <v>337</v>
@@ -34488,13 +34617,13 @@
         <v>337</v>
       </c>
       <c r="I2611" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2611" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="K2611" s="4">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="L2611" s="4">
         <v>225</v>
@@ -34512,7 +34641,7 @@
         <v>337</v>
       </c>
       <c r="F2612" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="G2612" s="4" t="s">
         <v>337</v>
@@ -34521,13 +34650,13 @@
         <v>337</v>
       </c>
       <c r="I2612" s="4">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="J2612" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="K2612" s="4">
-        <v>196</v>
+        <v>140</v>
       </c>
       <c r="L2612" s="4" t="s">
         <v>337</v>
@@ -34545,7 +34674,7 @@
         <v>337</v>
       </c>
       <c r="F2613" s="4">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="G2613" s="4" t="s">
         <v>337</v>
@@ -34554,13 +34683,13 @@
         <v>337</v>
       </c>
       <c r="I2613" s="4">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="J2613" s="4">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="K2613" s="4">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="L2613" s="4" t="s">
         <v>337</v>
@@ -34578,7 +34707,7 @@
         <v>337</v>
       </c>
       <c r="F2614" s="4">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="G2614" s="4" t="s">
         <v>337</v>
@@ -34587,13 +34716,13 @@
         <v>337</v>
       </c>
       <c r="I2614" s="4">
-        <v>159</v>
+        <v>103</v>
       </c>
       <c r="J2614" s="4">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="K2614" s="4">
-        <v>180</v>
+        <v>124</v>
       </c>
       <c r="L2614" s="4">
         <v>225</v>
@@ -34611,7 +34740,7 @@
         <v>337</v>
       </c>
       <c r="F2615" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2615" s="4" t="s">
         <v>337</v>
@@ -34620,13 +34749,13 @@
         <v>337</v>
       </c>
       <c r="I2615" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2615" s="4">
-        <v>173</v>
+        <v>117</v>
       </c>
       <c r="K2615" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2615" s="4" t="s">
         <v>337</v>
@@ -34644,7 +34773,7 @@
         <v>337</v>
       </c>
       <c r="F2616" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2616" s="4" t="s">
         <v>337</v>
@@ -34653,13 +34782,13 @@
         <v>337</v>
       </c>
       <c r="I2616" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2616" s="4">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="K2616" s="4">
-        <v>182</v>
+        <v>126</v>
       </c>
       <c r="L2616" s="4">
         <v>226</v>
@@ -34677,7 +34806,7 @@
         <v>337</v>
       </c>
       <c r="F2617" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2617" s="4" t="s">
         <v>337</v>
@@ -34686,13 +34815,13 @@
         <v>337</v>
       </c>
       <c r="I2617" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2617" s="4">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="K2617" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2617" s="4">
         <v>225</v>
@@ -34710,7 +34839,7 @@
         <v>337</v>
       </c>
       <c r="F2618" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2618" s="4" t="s">
         <v>337</v>
@@ -34719,13 +34848,13 @@
         <v>337</v>
       </c>
       <c r="I2618" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="J2618" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="K2618" s="4">
-        <v>192</v>
+        <v>136</v>
       </c>
       <c r="L2618" s="4" t="s">
         <v>337</v>
@@ -34743,7 +34872,7 @@
         <v>337</v>
       </c>
       <c r="F2619" s="4">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G2619" s="4" t="s">
         <v>337</v>
@@ -34752,13 +34881,13 @@
         <v>337</v>
       </c>
       <c r="I2619" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2619" s="4">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="K2619" s="4">
-        <v>179</v>
+        <v>123</v>
       </c>
       <c r="L2619" s="4">
         <v>225</v>
@@ -34776,7 +34905,7 @@
         <v>337</v>
       </c>
       <c r="F2620" s="4">
-        <v>161</v>
+        <v>105</v>
       </c>
       <c r="G2620" s="4" t="s">
         <v>337</v>
@@ -34785,13 +34914,13 @@
         <v>337</v>
       </c>
       <c r="I2620" s="4">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="J2620" s="4">
-        <v>177</v>
+        <v>121</v>
       </c>
       <c r="K2620" s="4">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="L2620" s="4">
         <v>226</v>
@@ -34809,7 +34938,7 @@
         <v>337</v>
       </c>
       <c r="F2621" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2621" s="4" t="s">
         <v>337</v>
@@ -34818,13 +34947,13 @@
         <v>337</v>
       </c>
       <c r="I2621" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="J2621" s="4">
-        <v>185</v>
+        <v>129</v>
       </c>
       <c r="K2621" s="4">
-        <v>189</v>
+        <v>133</v>
       </c>
       <c r="L2621" s="4" t="s">
         <v>337</v>
@@ -34842,7 +34971,7 @@
         <v>337</v>
       </c>
       <c r="F2622" s="4">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="G2622" s="4" t="s">
         <v>337</v>
@@ -34851,13 +34980,13 @@
         <v>337</v>
       </c>
       <c r="I2622" s="4">
-        <v>164</v>
+        <v>108</v>
       </c>
       <c r="J2622" s="4">
-        <v>171</v>
+        <v>115</v>
       </c>
       <c r="K2622" s="4">
-        <v>180</v>
+        <v>124</v>
       </c>
       <c r="L2622" s="4">
         <v>225</v>
@@ -34875,7 +35004,7 @@
         <v>337</v>
       </c>
       <c r="F2623" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="G2623" s="4" t="s">
         <v>337</v>
@@ -34884,13 +35013,13 @@
         <v>337</v>
       </c>
       <c r="I2623" s="4">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="J2623" s="4">
-        <v>181</v>
+        <v>125</v>
       </c>
       <c r="K2623" s="4">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="L2623" s="4" t="s">
         <v>337</v>
@@ -34908,7 +35037,7 @@
         <v>337</v>
       </c>
       <c r="F2624" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2624" s="4" t="s">
         <v>337</v>
@@ -34917,13 +35046,13 @@
         <v>337</v>
       </c>
       <c r="I2624" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2624" s="4">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="K2624" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2624" s="4" t="s">
         <v>337</v>
@@ -34941,7 +35070,7 @@
         <v>337</v>
       </c>
       <c r="F2625" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2625" s="4" t="s">
         <v>337</v>
@@ -34950,13 +35079,13 @@
         <v>337</v>
       </c>
       <c r="I2625" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2625" s="4">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="K2625" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2625" s="4">
         <v>225</v>
@@ -34974,7 +35103,7 @@
         <v>337</v>
       </c>
       <c r="F2626" s="4">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="G2626" s="4" t="s">
         <v>337</v>
@@ -34983,13 +35112,13 @@
         <v>337</v>
       </c>
       <c r="I2626" s="4">
-        <v>163</v>
+        <v>107</v>
       </c>
       <c r="J2626" s="4">
-        <v>176</v>
+        <v>120</v>
       </c>
       <c r="K2626" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2626" s="4">
         <v>225</v>
@@ -35007,7 +35136,7 @@
         <v>337</v>
       </c>
       <c r="F2627" s="4">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="G2627" s="4" t="s">
         <v>337</v>
@@ -35016,13 +35145,13 @@
         <v>337</v>
       </c>
       <c r="I2627" s="4">
-        <v>162</v>
+        <v>106</v>
       </c>
       <c r="J2627" s="4">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="K2627" s="4">
-        <v>184</v>
+        <v>128</v>
       </c>
       <c r="L2627" s="4">
         <v>226</v>

</xml_diff>